<commit_message>
fixed an error with pulling from same population
</commit_message>
<xml_diff>
--- a/Conference_2/conference_2_dataset.xlsx
+++ b/Conference_2/conference_2_dataset.xlsx
@@ -463,13 +463,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>84.76071649091432</v>
+        <v>72.94279470421998</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>27.90305466275058</v>
+        <v>36.70521453276492</v>
       </c>
     </row>
     <row r="3">
@@ -477,13 +477,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>67.53638274353676</v>
+        <v>92.07513949399892</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>44.11967502895164</v>
+        <v>32.02016550459801</v>
       </c>
     </row>
     <row r="4">
@@ -491,13 +491,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>77.12485851920974</v>
+        <v>66.36481864099747</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>34.4346013544554</v>
+        <v>29.89356029999565</v>
       </c>
     </row>
     <row r="5">
@@ -505,13 +505,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>67.23007435292364</v>
+        <v>70.80132505797864</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>48.80934472876939</v>
+        <v>22.84333043522985</v>
       </c>
     </row>
     <row r="6">
@@ -519,13 +519,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>66.47667746289855</v>
+        <v>75.52923515049392</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>60.1225446153301</v>
+        <v>34.79601976557151</v>
       </c>
     </row>
     <row r="7">
@@ -533,13 +533,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>67.65907180249522</v>
+        <v>84.14226772104226</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>18.46494396720312</v>
+        <v>48.78999146536775</v>
       </c>
     </row>
     <row r="8">
@@ -547,13 +547,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>75.66121244086177</v>
+        <v>66.93048072386676</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>39.71262963256051</v>
+        <v>34.52130393655413</v>
       </c>
     </row>
     <row r="9">
@@ -561,13 +561,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>82.01896762384939</v>
+        <v>71.42031821104256</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>44.27337254292743</v>
+        <v>16.12662187484598</v>
       </c>
     </row>
     <row r="10">
@@ -575,13 +575,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>82.86125959565329</v>
+        <v>76.40996908935965</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>47.33687342283091</v>
+        <v>31.54056571299223</v>
       </c>
     </row>
     <row r="11">
@@ -589,13 +589,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>62.74283683731199</v>
+        <v>68.44231085271822</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>35.85565564032454</v>
+        <v>49.364795240435</v>
       </c>
     </row>
     <row r="12">
@@ -603,13 +603,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>46.57727796104631</v>
+        <v>71.38915299214914</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>32.82870545962432</v>
+        <v>39.04005229776492</v>
       </c>
     </row>
     <row r="13">
@@ -617,13 +617,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>72.4970021275732</v>
+        <v>66.20053198256649</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>32.76131345823995</v>
+        <v>30.63042431316572</v>
       </c>
     </row>
     <row r="14">
@@ -631,13 +631,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>95.72544714356536</v>
+        <v>75.90812030802348</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>33.32622301387496</v>
+        <v>37.04216384696346</v>
       </c>
     </row>
     <row r="15">
@@ -645,13 +645,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>78.58538748463903</v>
+        <v>74.68415936845243</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>36.29010760063658</v>
+        <v>30.28706722664632</v>
       </c>
     </row>
     <row r="16">
@@ -659,13 +659,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>75.98411729842864</v>
+        <v>87.91956381419172</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>23.32892715198237</v>
+        <v>19.5845837131459</v>
       </c>
     </row>
     <row r="17">
@@ -673,13 +673,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>68.49831671650578</v>
+        <v>80.28745394549634</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>28.90390002368519</v>
+        <v>37.28623795067521</v>
       </c>
     </row>
     <row r="18">
@@ -687,13 +687,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>82.11544656226728</v>
+        <v>78.08022009846701</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>23.37332312880626</v>
+        <v>24.76171028779522</v>
       </c>
     </row>
     <row r="19">
@@ -701,13 +701,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>75.82464418097027</v>
+        <v>73.96219400535186</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>35.41689413700468</v>
+        <v>26.97913864652084</v>
       </c>
     </row>
     <row r="20">
@@ -715,13 +715,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>91.14543211938505</v>
+        <v>80.49631159313969</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>37.96133484636049</v>
+        <v>28.06327556786315</v>
       </c>
     </row>
     <row r="21">
@@ -729,13 +729,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>74.24276693381499</v>
+        <v>73.8852121965493</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>42.86874352968093</v>
+        <v>45.13689773323661</v>
       </c>
     </row>
     <row r="22">
@@ -743,13 +743,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>84.7070162965255</v>
+        <v>74.53340279876228</v>
       </c>
       <c r="C22" t="n">
         <v>21</v>
       </c>
       <c r="D22" t="n">
-        <v>21.58583084018648</v>
+        <v>22.98771031615451</v>
       </c>
     </row>
     <row r="23">
@@ -757,13 +757,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>58.86042150373672</v>
+        <v>78.70958252950098</v>
       </c>
       <c r="C23" t="n">
         <v>22</v>
       </c>
       <c r="D23" t="n">
-        <v>49.43506166330805</v>
+        <v>37.73579738086963</v>
       </c>
     </row>
     <row r="24">
@@ -771,13 +771,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>70.17587422899253</v>
+        <v>75.9130635606336</v>
       </c>
       <c r="C24" t="n">
         <v>23</v>
       </c>
       <c r="D24" t="n">
-        <v>53.7982293283055</v>
+        <v>15.16280715492885</v>
       </c>
     </row>
     <row r="25">
@@ -785,13 +785,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>75.62344335973222</v>
+        <v>71.59380225242441</v>
       </c>
       <c r="C25" t="n">
         <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>36.06925667173261</v>
+        <v>27.49531133358101</v>
       </c>
     </row>
     <row r="26">
@@ -799,13 +799,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>78.27228349950755</v>
+        <v>95.3793667518153</v>
       </c>
       <c r="C26" t="n">
         <v>25</v>
       </c>
       <c r="D26" t="n">
-        <v>28.31389779462784</v>
+        <v>18.75242264745681</v>
       </c>
     </row>
   </sheetData>
@@ -854,13 +854,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>7857.850364130243</v>
+        <v>7353.215594055656</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>7390.136662972348</v>
+        <v>7762.713071321208</v>
       </c>
     </row>
     <row r="3">
@@ -868,13 +868,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>7677.143694515695</v>
+        <v>7975.790646420667</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>7821.773548721154</v>
+        <v>7876.558190783439</v>
       </c>
     </row>
     <row r="4">
@@ -882,13 +882,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>7506.848394102688</v>
+        <v>7660.713953724737</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>7809.709565881628</v>
+        <v>7769.511782434512</v>
       </c>
     </row>
     <row r="5">
@@ -896,13 +896,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>7248.329398616952</v>
+        <v>7639.031460796443</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>7489.796937802614</v>
+        <v>7722.595458136684</v>
       </c>
     </row>
     <row r="6">
@@ -910,13 +910,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>7687.100323181082</v>
+        <v>7147.883187928498</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>7202.956534609439</v>
+        <v>7796.570913263394</v>
       </c>
     </row>
     <row r="7">
@@ -924,13 +924,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>7230.690542915488</v>
+        <v>7260.943145493006</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>7796.073373474883</v>
+        <v>7752.830441209841</v>
       </c>
     </row>
     <row r="8">
@@ -938,13 +938,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>7711.825866510662</v>
+        <v>7844.198236024468</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>7801.626557241434</v>
+        <v>7884.706960983995</v>
       </c>
     </row>
     <row r="9">
@@ -952,13 +952,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>7793.193122104441</v>
+        <v>7819.014104057161</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>7186.493653704789</v>
+        <v>7801.446618174664</v>
       </c>
     </row>
     <row r="10">
@@ -966,13 +966,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>7941.174559785502</v>
+        <v>7732.101687579802</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>7856.128502383094</v>
+        <v>7849.710632886737</v>
       </c>
     </row>
     <row r="11">
@@ -980,13 +980,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>7867.692247056333</v>
+        <v>7827.245640768148</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>7795.089493117952</v>
+        <v>7890.636203354271</v>
       </c>
     </row>
     <row r="12">
@@ -994,13 +994,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>7591.148922607396</v>
+        <v>7242.002308227853</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>7779.701108029407</v>
+        <v>7157.382178107472</v>
       </c>
     </row>
     <row r="13">
@@ -1008,13 +1008,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>7950.41456766604</v>
+        <v>7588.245895762215</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>7901.649860648576</v>
+        <v>6931.597172885003</v>
       </c>
     </row>
     <row r="14">
@@ -1022,13 +1022,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>7946.833522378316</v>
+        <v>7545.433086295076</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>7315.384548692318</v>
+        <v>7634.154515075037</v>
       </c>
     </row>
     <row r="15">
@@ -1036,13 +1036,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>7324.500031755955</v>
+        <v>7211.774757964048</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>7904.535035963735</v>
+        <v>7759.718818612501</v>
       </c>
     </row>
     <row r="16">
@@ -1050,13 +1050,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>7735.884135382954</v>
+        <v>7946.584217243846</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>7310.141901245536</v>
+        <v>7913.268622579293</v>
       </c>
     </row>
     <row r="17">
@@ -1064,13 +1064,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>7737.463102407796</v>
+        <v>7352.120855946994</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>6755.956491719546</v>
+        <v>7202.200891091383</v>
       </c>
     </row>
     <row r="18">
@@ -1078,13 +1078,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>7404.902917094713</v>
+        <v>7926.253928277662</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>6858.845128353544</v>
+        <v>7982.969243851872</v>
       </c>
     </row>
     <row r="19">
@@ -1092,13 +1092,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>7457.665653143441</v>
+        <v>7609.756144418237</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>7883.445210770324</v>
+        <v>7375.467150100754</v>
       </c>
     </row>
     <row r="20">
@@ -1106,13 +1106,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>7885.261963488034</v>
+        <v>7942.415360415031</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>7909.949072509548</v>
+        <v>7162.278032980534</v>
       </c>
     </row>
     <row r="21">
@@ -1120,13 +1120,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>7273.341206397633</v>
+        <v>7707.730167716622</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>7743.78334171744</v>
+        <v>7072.051111625772</v>
       </c>
     </row>
   </sheetData>
@@ -1140,7 +1140,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1175,13 +1175,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.835553860566018</v>
+        <v>0.8377150399607347</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7909200354818077</v>
+        <v>0.5948922502548245</v>
       </c>
     </row>
     <row r="3">
@@ -1189,13 +1189,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.9727273326232251</v>
+        <v>0.8988391168649432</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5733898968330832</v>
+        <v>0.551381686497301</v>
       </c>
     </row>
     <row r="4">
@@ -1203,13 +1203,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.4089460055647117</v>
+        <v>0.8749937801909435</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>0.139080922146308</v>
+        <v>0.5371977348458755</v>
       </c>
     </row>
     <row r="5">
@@ -1217,13 +1217,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.3659755003316322</v>
+        <v>0.829834381265377</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9284497198146536</v>
+        <v>0.5651222082897059</v>
       </c>
     </row>
     <row r="6">
@@ -1231,13 +1231,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2646248680166002</v>
+        <v>0.8886302275842173</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6109852446583856</v>
+        <v>0.5363389456764688</v>
       </c>
     </row>
     <row r="7">
@@ -1245,13 +1245,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9627625531414657</v>
+        <v>0.8741547420439911</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5854151261273842</v>
+        <v>0.5283667234617535</v>
       </c>
     </row>
     <row r="8">
@@ -1259,13 +1259,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.01623800898701289</v>
+        <v>0.8671734023163128</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1124202792914301</v>
+        <v>0.5265060374781659</v>
       </c>
     </row>
     <row r="9">
@@ -1273,13 +1273,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.7856791483378753</v>
+        <v>0.811397099621575</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>0.721565628767859</v>
+        <v>0.5337429366804486</v>
       </c>
     </row>
     <row r="10">
@@ -1287,13 +1287,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.8577479982680514</v>
+        <v>0.8162525210011262</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>0.8407582986092303</v>
+        <v>0.5017279996254543</v>
       </c>
     </row>
     <row r="11">
@@ -1301,13 +1301,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.3852138288766448</v>
+        <v>0.8566247721483311</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5269371494185077</v>
+        <v>0.585080737353125</v>
       </c>
     </row>
     <row r="12">
@@ -1315,13 +1315,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>0.9692115057012375</v>
+        <v>0.8506566464335196</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>0.2323998276010369</v>
+        <v>0.5081033831344123</v>
       </c>
     </row>
     <row r="13">
@@ -1329,13 +1329,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>0.7239855008202716</v>
+        <v>0.8941094886933617</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>0.2769213269683342</v>
+        <v>0.5717155965472498</v>
       </c>
     </row>
     <row r="14">
@@ -1343,13 +1343,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.002190547551095934</v>
+        <v>0.8951347970335071</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>0.3284289977324477</v>
+        <v>0.5750525513347545</v>
       </c>
     </row>
     <row r="15">
@@ -1357,13 +1357,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.2412214060831597</v>
+        <v>0.8532606554204418</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>0.8060773477841775</v>
+        <v>0.5133301929991114</v>
       </c>
     </row>
     <row r="16">
@@ -1371,13 +1371,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>0.5616624282537276</v>
+        <v>0.8831008314701528</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>0.264317110229484</v>
+        <v>0.5533292207632123</v>
       </c>
     </row>
     <row r="17">
@@ -1385,13 +1385,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>0.3289280204745976</v>
+        <v>0.8940862779541737</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0458932728017527</v>
+        <v>0.5311645171825924</v>
       </c>
     </row>
     <row r="18">
@@ -1399,13 +1399,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>0.9710811408915304</v>
+        <v>0.8041693043972526</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>0.3040621447964249</v>
+        <v>0.5770375469352905</v>
       </c>
     </row>
     <row r="19">
@@ -1413,13 +1413,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>0.2599741751328061</v>
+        <v>0.8228638867129748</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>0.786184290870142</v>
+        <v>0.5719691448725772</v>
       </c>
     </row>
     <row r="20">
@@ -1427,13 +1427,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>0.2015627022666848</v>
+        <v>0.8431538155626279</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>0.816832503058013</v>
+        <v>0.5466784272934183</v>
       </c>
     </row>
     <row r="21">
@@ -1441,13 +1441,293 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>0.3617853718864176</v>
+        <v>0.8435608830866178</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>0.4984146583264599</v>
+        <v>0.5706664601364493</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.8694313645769924</v>
+      </c>
+      <c r="C22" t="n">
+        <v>21</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.5641796931762271</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.8207867597901592</v>
+      </c>
+      <c r="C23" t="n">
+        <v>22</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.5421352120983041</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.8505257953431904</v>
+      </c>
+      <c r="C24" t="n">
+        <v>23</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.57886441440584</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.8010704362205588</v>
+      </c>
+      <c r="C25" t="n">
+        <v>24</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.5358780460727206</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.8588595723336664</v>
+      </c>
+      <c r="C26" t="n">
+        <v>25</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.5068957534529337</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0.8388950595733562</v>
+      </c>
+      <c r="C27" t="n">
+        <v>26</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.5697436333479138</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.8117387056288498</v>
+      </c>
+      <c r="C28" t="n">
+        <v>27</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.585618207990664</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.8154825032863551</v>
+      </c>
+      <c r="C29" t="n">
+        <v>28</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.5869747974047627</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0.8317276674299148</v>
+      </c>
+      <c r="C30" t="n">
+        <v>29</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.565636209385828</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.892749161978371</v>
+      </c>
+      <c r="C31" t="n">
+        <v>30</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.5564881735190295</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.8382618263765373</v>
+      </c>
+      <c r="C32" t="n">
+        <v>31</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.5621260551147569</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0.8438772641428293</v>
+      </c>
+      <c r="C33" t="n">
+        <v>32</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.5371979688043156</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0.8544846021101352</v>
+      </c>
+      <c r="C34" t="n">
+        <v>33</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.5307233888318081</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0.8888404931075737</v>
+      </c>
+      <c r="C35" t="n">
+        <v>34</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.5439161848763482</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0.8972202980894219</v>
+      </c>
+      <c r="C36" t="n">
+        <v>35</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.5924907367345024</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0.8316713779197955</v>
+      </c>
+      <c r="C37" t="n">
+        <v>36</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.5137427208956106</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0.8492599528521483</v>
+      </c>
+      <c r="C38" t="n">
+        <v>37</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.5893859735783338</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0.855388506601937</v>
+      </c>
+      <c r="C39" t="n">
+        <v>38</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.5239753680295947</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.8725942932822429</v>
+      </c>
+      <c r="C40" t="n">
+        <v>39</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.5863003530349391</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0.8621861531131386</v>
+      </c>
+      <c r="C41" t="n">
+        <v>40</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.5195239798295231</v>
       </c>
     </row>
   </sheetData>
@@ -1510,13 +1790,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
@@ -1524,13 +1804,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
@@ -1544,7 +1824,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
@@ -1552,13 +1832,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
@@ -1566,13 +1846,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -1580,13 +1860,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
@@ -1594,13 +1874,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
@@ -1608,13 +1888,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
@@ -1622,13 +1902,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12">
@@ -1636,13 +1916,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
@@ -1664,13 +1944,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15">
@@ -1678,7 +1958,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
@@ -1692,13 +1972,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17">
@@ -1706,13 +1986,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18">
@@ -1720,13 +2000,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19">
@@ -1734,7 +2014,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
@@ -1748,13 +2028,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21">
@@ -1762,13 +2042,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
@@ -1776,13 +2056,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C22" t="n">
         <v>21</v>
       </c>
       <c r="D22" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23">
@@ -1790,13 +2070,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C23" t="n">
         <v>22</v>
       </c>
       <c r="D23" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24">
@@ -1804,13 +2084,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C24" t="n">
         <v>23</v>
       </c>
       <c r="D24" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25">
@@ -1818,7 +2098,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C25" t="n">
         <v>24</v>
@@ -1832,13 +2112,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C26" t="n">
         <v>25</v>
       </c>
       <c r="D26" t="n">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
horse data still returning normal
</commit_message>
<xml_diff>
--- a/Conference_2/conference_2_dataset.xlsx
+++ b/Conference_2/conference_2_dataset.xlsx
@@ -463,13 +463,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>72.94279470421998</v>
+        <v>65.03006435068491</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>36.70521453276492</v>
+        <v>29.55041064900904</v>
       </c>
     </row>
     <row r="3">
@@ -477,13 +477,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>92.07513949399892</v>
+        <v>69.71579494095644</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>32.02016550459801</v>
+        <v>26.68076925813271</v>
       </c>
     </row>
     <row r="4">
@@ -491,13 +491,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>66.36481864099747</v>
+        <v>75.74370108163872</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>29.89356029999565</v>
+        <v>47.81926196778836</v>
       </c>
     </row>
     <row r="5">
@@ -505,13 +505,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>70.80132505797864</v>
+        <v>83.09707998985907</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>22.84333043522985</v>
+        <v>27.96391793671203</v>
       </c>
     </row>
     <row r="6">
@@ -519,13 +519,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>75.52923515049392</v>
+        <v>63.7186528847603</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>34.79601976557151</v>
+        <v>37.79609048470516</v>
       </c>
     </row>
     <row r="7">
@@ -533,13 +533,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>84.14226772104226</v>
+        <v>71.23479869481011</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>48.78999146536775</v>
+        <v>25.31468801903539</v>
       </c>
     </row>
     <row r="8">
@@ -547,13 +547,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>66.93048072386676</v>
+        <v>73.61731565259345</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>34.52130393655413</v>
+        <v>20.82191331595294</v>
       </c>
     </row>
     <row r="9">
@@ -561,13 +561,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>71.42031821104256</v>
+        <v>70.78146322440479</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>16.12662187484598</v>
+        <v>50.16767119380519</v>
       </c>
     </row>
     <row r="10">
@@ -575,13 +575,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>76.40996908935965</v>
+        <v>87.74275285989015</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>31.54056571299223</v>
+        <v>37.01703345467151</v>
       </c>
     </row>
     <row r="11">
@@ -589,13 +589,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>68.44231085271822</v>
+        <v>65.07725777705893</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>49.364795240435</v>
+        <v>18.92773769807461</v>
       </c>
     </row>
     <row r="12">
@@ -603,13 +603,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>71.38915299214914</v>
+        <v>84.18389461883854</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>39.04005229776492</v>
+        <v>32.48013797558948</v>
       </c>
     </row>
     <row r="13">
@@ -617,13 +617,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>66.20053198256649</v>
+        <v>84.09769116136376</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>30.63042431316572</v>
+        <v>42.10087373196664</v>
       </c>
     </row>
     <row r="14">
@@ -631,13 +631,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>75.90812030802348</v>
+        <v>53.41095777554392</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>37.04216384696346</v>
+        <v>46.70020264959377</v>
       </c>
     </row>
     <row r="15">
@@ -645,13 +645,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>74.68415936845243</v>
+        <v>76.80863064009743</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>30.28706722664632</v>
+        <v>30.27835830246625</v>
       </c>
     </row>
     <row r="16">
@@ -659,13 +659,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>87.91956381419172</v>
+        <v>72.20924158141578</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>19.5845837131459</v>
+        <v>37.47606163303947</v>
       </c>
     </row>
     <row r="17">
@@ -673,13 +673,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>80.28745394549634</v>
+        <v>63.4947953640909</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>37.28623795067521</v>
+        <v>20.22874134428619</v>
       </c>
     </row>
     <row r="18">
@@ -687,13 +687,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>78.08022009846701</v>
+        <v>86.50680160591641</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>24.76171028779522</v>
+        <v>43.79122922720687</v>
       </c>
     </row>
     <row r="19">
@@ -701,13 +701,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>73.96219400535186</v>
+        <v>78.28930487092752</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>26.97913864652084</v>
+        <v>26.19318912777108</v>
       </c>
     </row>
     <row r="20">
@@ -715,13 +715,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>80.49631159313969</v>
+        <v>61.16937452653605</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>28.06327556786315</v>
+        <v>33.29926720781165</v>
       </c>
     </row>
     <row r="21">
@@ -729,13 +729,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>73.8852121965493</v>
+        <v>65.35430493132003</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>45.13689773323661</v>
+        <v>44.35265564626028</v>
       </c>
     </row>
     <row r="22">
@@ -743,13 +743,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>74.53340279876228</v>
+        <v>82.2215658668943</v>
       </c>
       <c r="C22" t="n">
         <v>21</v>
       </c>
       <c r="D22" t="n">
-        <v>22.98771031615451</v>
+        <v>38.23854664125035</v>
       </c>
     </row>
     <row r="23">
@@ -757,13 +757,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>78.70958252950098</v>
+        <v>68.78449716220743</v>
       </c>
       <c r="C23" t="n">
         <v>22</v>
       </c>
       <c r="D23" t="n">
-        <v>37.73579738086963</v>
+        <v>34.26100335248395</v>
       </c>
     </row>
     <row r="24">
@@ -771,13 +771,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>75.9130635606336</v>
+        <v>62.84382071551743</v>
       </c>
       <c r="C24" t="n">
         <v>23</v>
       </c>
       <c r="D24" t="n">
-        <v>15.16280715492885</v>
+        <v>45.07265708968812</v>
       </c>
     </row>
     <row r="25">
@@ -785,13 +785,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>71.59380225242441</v>
+        <v>61.39654528798138</v>
       </c>
       <c r="C25" t="n">
         <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>27.49531133358101</v>
+        <v>33.55445371607875</v>
       </c>
     </row>
     <row r="26">
@@ -799,13 +799,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>95.3793667518153</v>
+        <v>74.51230855430882</v>
       </c>
       <c r="C26" t="n">
         <v>25</v>
       </c>
       <c r="D26" t="n">
-        <v>18.75242264745681</v>
+        <v>46.80194324645724</v>
       </c>
     </row>
   </sheetData>
@@ -854,13 +854,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>7353.215594055656</v>
+        <v>7670.849727980974</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>7762.713071321208</v>
+        <v>7786.008131453756</v>
       </c>
     </row>
     <row r="3">
@@ -868,13 +868,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>7975.790646420667</v>
+        <v>7839.553860100211</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>7876.558190783439</v>
+        <v>7930.746276599633</v>
       </c>
     </row>
     <row r="4">
@@ -882,13 +882,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>7660.713953724737</v>
+        <v>7896.986428762432</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>7769.511782434512</v>
+        <v>7635.411153064268</v>
       </c>
     </row>
     <row r="5">
@@ -896,13 +896,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>7639.031460796443</v>
+        <v>6736.420690021456</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>7722.595458136684</v>
+        <v>6738.798679690955</v>
       </c>
     </row>
     <row r="6">
@@ -910,13 +910,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>7147.883187928498</v>
+        <v>7869.557453601535</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>7796.570913263394</v>
+        <v>7843.069961535311</v>
       </c>
     </row>
     <row r="7">
@@ -924,13 +924,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>7260.943145493006</v>
+        <v>7046.854857798955</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>7752.830441209841</v>
+        <v>7868.352659180621</v>
       </c>
     </row>
     <row r="8">
@@ -938,13 +938,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>7844.198236024468</v>
+        <v>7775.476429794619</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>7884.706960983995</v>
+        <v>7696.245592668011</v>
       </c>
     </row>
     <row r="9">
@@ -952,13 +952,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>7819.014104057161</v>
+        <v>7755.924873889781</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>7801.446618174664</v>
+        <v>7761.573699518959</v>
       </c>
     </row>
     <row r="10">
@@ -966,13 +966,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>7732.101687579802</v>
+        <v>7591.248917543384</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>7849.710632886737</v>
+        <v>7266.450565672319</v>
       </c>
     </row>
     <row r="11">
@@ -980,13 +980,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>7827.245640768148</v>
+        <v>7631.941456554055</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>7890.636203354271</v>
+        <v>7881.859499700697</v>
       </c>
     </row>
     <row r="12">
@@ -994,13 +994,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>7242.002308227853</v>
+        <v>7082.025346454595</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>7157.382178107472</v>
+        <v>7365.598187607988</v>
       </c>
     </row>
     <row r="13">
@@ -1008,13 +1008,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>7588.245895762215</v>
+        <v>7381.660580233637</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>6931.597172885003</v>
+        <v>7751.166957167938</v>
       </c>
     </row>
     <row r="14">
@@ -1022,13 +1022,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>7545.433086295076</v>
+        <v>7624.744707497926</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>7634.154515075037</v>
+        <v>7918.685829140993</v>
       </c>
     </row>
     <row r="15">
@@ -1036,13 +1036,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>7211.774757964048</v>
+        <v>6499.744225423534</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>7759.718818612501</v>
+        <v>7320.772646146371</v>
       </c>
     </row>
     <row r="16">
@@ -1050,13 +1050,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>7946.584217243846</v>
+        <v>7901.897751089019</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>7913.268622579293</v>
+        <v>7572.168701810511</v>
       </c>
     </row>
     <row r="17">
@@ -1064,13 +1064,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>7352.120855946994</v>
+        <v>7321.041986935189</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>7202.200891091383</v>
+        <v>7104.112623935078</v>
       </c>
     </row>
     <row r="18">
@@ -1078,13 +1078,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>7926.253928277662</v>
+        <v>7669.954099645398</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>7982.969243851872</v>
+        <v>7901.469787517514</v>
       </c>
     </row>
     <row r="19">
@@ -1092,13 +1092,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>7609.756144418237</v>
+        <v>7866.154589076468</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>7375.467150100754</v>
+        <v>6861.10383664087</v>
       </c>
     </row>
     <row r="20">
@@ -1106,13 +1106,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>7942.415360415031</v>
+        <v>7982.216554077999</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>7162.278032980534</v>
+        <v>6753.399774018735</v>
       </c>
     </row>
     <row r="21">
@@ -1120,13 +1120,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>7707.730167716622</v>
+        <v>7486.859344583012</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>7072.051111625772</v>
+        <v>7775.520950329103</v>
       </c>
     </row>
   </sheetData>
@@ -1175,13 +1175,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.8377150399607347</v>
+        <v>0.8669000418115111</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5948922502548245</v>
+        <v>0.5344816371220522</v>
       </c>
     </row>
     <row r="3">
@@ -1189,13 +1189,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8988391168649432</v>
+        <v>0.8111448160986828</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>0.551381686497301</v>
+        <v>0.5018545418826674</v>
       </c>
     </row>
     <row r="4">
@@ -1203,13 +1203,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8749937801909435</v>
+        <v>0.866390509303972</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5371977348458755</v>
+        <v>0.5244599367168462</v>
       </c>
     </row>
     <row r="5">
@@ -1217,13 +1217,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.829834381265377</v>
+        <v>0.8343524574238459</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5651222082897059</v>
+        <v>0.5193582296050649</v>
       </c>
     </row>
     <row r="6">
@@ -1231,13 +1231,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8886302275842173</v>
+        <v>0.8669649014059136</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5363389456764688</v>
+        <v>0.5266023898763372</v>
       </c>
     </row>
     <row r="7">
@@ -1245,13 +1245,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.8741547420439911</v>
+        <v>0.8363924618911617</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5283667234617535</v>
+        <v>0.5923377031738626</v>
       </c>
     </row>
     <row r="8">
@@ -1259,13 +1259,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.8671734023163128</v>
+        <v>0.8233685019279536</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5265060374781659</v>
+        <v>0.5081204926888248</v>
       </c>
     </row>
     <row r="9">
@@ -1273,13 +1273,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.811397099621575</v>
+        <v>0.8726878039822333</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5337429366804486</v>
+        <v>0.5834013385360847</v>
       </c>
     </row>
     <row r="10">
@@ -1287,13 +1287,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.8162525210011262</v>
+        <v>0.8552210796272611</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5017279996254543</v>
+        <v>0.5019660249534544</v>
       </c>
     </row>
     <row r="11">
@@ -1301,13 +1301,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.8566247721483311</v>
+        <v>0.89716609122131</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>0.585080737353125</v>
+        <v>0.5028313524348221</v>
       </c>
     </row>
     <row r="12">
@@ -1315,13 +1315,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>0.8506566464335196</v>
+        <v>0.8709698695777164</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5081033831344123</v>
+        <v>0.5962914138674927</v>
       </c>
     </row>
     <row r="13">
@@ -1329,13 +1329,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>0.8941094886933617</v>
+        <v>0.83157529835301</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5717155965472498</v>
+        <v>0.5539081401270842</v>
       </c>
     </row>
     <row r="14">
@@ -1343,13 +1343,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.8951347970335071</v>
+        <v>0.8211682856157061</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5750525513347545</v>
+        <v>0.5474254482241685</v>
       </c>
     </row>
     <row r="15">
@@ -1357,13 +1357,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.8532606554204418</v>
+        <v>0.8240967467226784</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5133301929991114</v>
+        <v>0.5919359941631341</v>
       </c>
     </row>
     <row r="16">
@@ -1371,13 +1371,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>0.8831008314701528</v>
+        <v>0.8289548331299081</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>0.5533292207632123</v>
+        <v>0.5536565663790451</v>
       </c>
     </row>
     <row r="17">
@@ -1385,13 +1385,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>0.8940862779541737</v>
+        <v>0.8621366096020281</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5311645171825924</v>
+        <v>0.5230679692918924</v>
       </c>
     </row>
     <row r="18">
@@ -1399,13 +1399,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>0.8041693043972526</v>
+        <v>0.8944371439060989</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5770375469352905</v>
+        <v>0.5841997097660503</v>
       </c>
     </row>
     <row r="19">
@@ -1413,13 +1413,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>0.8228638867129748</v>
+        <v>0.8970864450667373</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>0.5719691448725772</v>
+        <v>0.5909989160872702</v>
       </c>
     </row>
     <row r="20">
@@ -1427,13 +1427,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>0.8431538155626279</v>
+        <v>0.8939511512807504</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>0.5466784272934183</v>
+        <v>0.5011323243985301</v>
       </c>
     </row>
     <row r="21">
@@ -1441,13 +1441,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>0.8435608830866178</v>
+        <v>0.886760507231459</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5706664601364493</v>
+        <v>0.5537661016152468</v>
       </c>
     </row>
     <row r="22">
@@ -1455,13 +1455,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>0.8694313645769924</v>
+        <v>0.8862258104538903</v>
       </c>
       <c r="C22" t="n">
         <v>21</v>
       </c>
       <c r="D22" t="n">
-        <v>0.5641796931762271</v>
+        <v>0.576069603779173</v>
       </c>
     </row>
     <row r="23">
@@ -1469,13 +1469,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>0.8207867597901592</v>
+        <v>0.8194186760563227</v>
       </c>
       <c r="C23" t="n">
         <v>22</v>
       </c>
       <c r="D23" t="n">
-        <v>0.5421352120983041</v>
+        <v>0.5824252951294644</v>
       </c>
     </row>
     <row r="24">
@@ -1483,13 +1483,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>0.8505257953431904</v>
+        <v>0.8303386517533771</v>
       </c>
       <c r="C24" t="n">
         <v>23</v>
       </c>
       <c r="D24" t="n">
-        <v>0.57886441440584</v>
+        <v>0.5768870941784824</v>
       </c>
     </row>
     <row r="25">
@@ -1497,13 +1497,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>0.8010704362205588</v>
+        <v>0.8094030056144252</v>
       </c>
       <c r="C25" t="n">
         <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>0.5358780460727206</v>
+        <v>0.5106677397729527</v>
       </c>
     </row>
     <row r="26">
@@ -1511,13 +1511,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>0.8588595723336664</v>
+        <v>0.8417678346249561</v>
       </c>
       <c r="C26" t="n">
         <v>25</v>
       </c>
       <c r="D26" t="n">
-        <v>0.5068957534529337</v>
+        <v>0.5241948481021546</v>
       </c>
     </row>
     <row r="27">
@@ -1525,13 +1525,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>0.8388950595733562</v>
+        <v>0.8354107523962944</v>
       </c>
       <c r="C27" t="n">
         <v>26</v>
       </c>
       <c r="D27" t="n">
-        <v>0.5697436333479138</v>
+        <v>0.5903434150491226</v>
       </c>
     </row>
     <row r="28">
@@ -1539,13 +1539,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>0.8117387056288498</v>
+        <v>0.8893642414095376</v>
       </c>
       <c r="C28" t="n">
         <v>27</v>
       </c>
       <c r="D28" t="n">
-        <v>0.585618207990664</v>
+        <v>0.554751323035479</v>
       </c>
     </row>
     <row r="29">
@@ -1553,13 +1553,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>0.8154825032863551</v>
+        <v>0.8133459655823825</v>
       </c>
       <c r="C29" t="n">
         <v>28</v>
       </c>
       <c r="D29" t="n">
-        <v>0.5869747974047627</v>
+        <v>0.5349588467409012</v>
       </c>
     </row>
     <row r="30">
@@ -1567,13 +1567,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>0.8317276674299148</v>
+        <v>0.8608056037748639</v>
       </c>
       <c r="C30" t="n">
         <v>29</v>
       </c>
       <c r="D30" t="n">
-        <v>0.565636209385828</v>
+        <v>0.5671532254619741</v>
       </c>
     </row>
     <row r="31">
@@ -1581,13 +1581,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>0.892749161978371</v>
+        <v>0.8186369116592933</v>
       </c>
       <c r="C31" t="n">
         <v>30</v>
       </c>
       <c r="D31" t="n">
-        <v>0.5564881735190295</v>
+        <v>0.5404886120693058</v>
       </c>
     </row>
     <row r="32">
@@ -1595,13 +1595,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>0.8382618263765373</v>
+        <v>0.8232446756988376</v>
       </c>
       <c r="C32" t="n">
         <v>31</v>
       </c>
       <c r="D32" t="n">
-        <v>0.5621260551147569</v>
+        <v>0.5172487217728502</v>
       </c>
     </row>
     <row r="33">
@@ -1609,13 +1609,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>0.8438772641428293</v>
+        <v>0.8291769694151093</v>
       </c>
       <c r="C33" t="n">
         <v>32</v>
       </c>
       <c r="D33" t="n">
-        <v>0.5371979688043156</v>
+        <v>0.5041364146982324</v>
       </c>
     </row>
     <row r="34">
@@ -1623,13 +1623,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>0.8544846021101352</v>
+        <v>0.8311120790166713</v>
       </c>
       <c r="C34" t="n">
         <v>33</v>
       </c>
       <c r="D34" t="n">
-        <v>0.5307233888318081</v>
+        <v>0.5698087597126311</v>
       </c>
     </row>
     <row r="35">
@@ -1637,13 +1637,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>0.8888404931075737</v>
+        <v>0.885214558986105</v>
       </c>
       <c r="C35" t="n">
         <v>34</v>
       </c>
       <c r="D35" t="n">
-        <v>0.5439161848763482</v>
+        <v>0.5267040774995533</v>
       </c>
     </row>
     <row r="36">
@@ -1651,13 +1651,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>0.8972202980894219</v>
+        <v>0.8549856502986842</v>
       </c>
       <c r="C36" t="n">
         <v>35</v>
       </c>
       <c r="D36" t="n">
-        <v>0.5924907367345024</v>
+        <v>0.5054224103846067</v>
       </c>
     </row>
     <row r="37">
@@ -1665,13 +1665,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>0.8316713779197955</v>
+        <v>0.8589022566631083</v>
       </c>
       <c r="C37" t="n">
         <v>36</v>
       </c>
       <c r="D37" t="n">
-        <v>0.5137427208956106</v>
+        <v>0.5171754412046695</v>
       </c>
     </row>
     <row r="38">
@@ -1679,13 +1679,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>0.8492599528521483</v>
+        <v>0.86516146997175</v>
       </c>
       <c r="C38" t="n">
         <v>37</v>
       </c>
       <c r="D38" t="n">
-        <v>0.5893859735783338</v>
+        <v>0.5970111276673999</v>
       </c>
     </row>
     <row r="39">
@@ -1693,13 +1693,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>0.855388506601937</v>
+        <v>0.8104532239530559</v>
       </c>
       <c r="C39" t="n">
         <v>38</v>
       </c>
       <c r="D39" t="n">
-        <v>0.5239753680295947</v>
+        <v>0.5454447961603374</v>
       </c>
     </row>
     <row r="40">
@@ -1707,13 +1707,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>0.8725942932822429</v>
+        <v>0.8879369800786422</v>
       </c>
       <c r="C40" t="n">
         <v>39</v>
       </c>
       <c r="D40" t="n">
-        <v>0.5863003530349391</v>
+        <v>0.5065508412852862</v>
       </c>
     </row>
     <row r="41">
@@ -1721,13 +1721,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>0.8621861531131386</v>
+        <v>0.803322716392506</v>
       </c>
       <c r="C41" t="n">
         <v>40</v>
       </c>
       <c r="D41" t="n">
-        <v>0.5195239798295231</v>
+        <v>0.5930523726155574</v>
       </c>
     </row>
   </sheetData>
@@ -1776,13 +1776,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
@@ -1790,13 +1790,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -1804,7 +1804,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
@@ -1824,7 +1824,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
@@ -1838,7 +1838,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
@@ -1846,13 +1846,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
@@ -1860,13 +1860,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
@@ -1874,13 +1874,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10">
@@ -1888,13 +1888,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
@@ -1902,13 +1902,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12">
@@ -1916,13 +1916,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
@@ -1930,13 +1930,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
@@ -1950,7 +1950,7 @@
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15">
@@ -1958,13 +1958,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16">
@@ -1972,13 +1972,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17">
@@ -1986,13 +1986,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18">
@@ -2000,7 +2000,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
@@ -2014,13 +2014,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20">
@@ -2028,13 +2028,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21">
@@ -2042,13 +2042,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22">
@@ -2062,7 +2062,7 @@
         <v>21</v>
       </c>
       <c r="D22" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23">
@@ -2070,13 +2070,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C23" t="n">
         <v>22</v>
       </c>
       <c r="D23" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24">
@@ -2084,13 +2084,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C24" t="n">
         <v>23</v>
       </c>
       <c r="D24" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25">
@@ -2098,13 +2098,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25" t="n">
         <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26">
@@ -2112,7 +2112,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" t="n">
         <v>25</v>

</xml_diff>

<commit_message>
fixed an error with not normal data
</commit_message>
<xml_diff>
--- a/Conference_2/conference_2_dataset.xlsx
+++ b/Conference_2/conference_2_dataset.xlsx
@@ -463,13 +463,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>65.03006435068491</v>
+        <v>78.66517198604831</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>29.55041064900904</v>
+        <v>9.571141800408675</v>
       </c>
     </row>
     <row r="3">
@@ -477,13 +477,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>69.71579494095644</v>
+        <v>84.59987674157436</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>26.68076925813271</v>
+        <v>33.23424685252404</v>
       </c>
     </row>
     <row r="4">
@@ -491,13 +491,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>75.74370108163872</v>
+        <v>73.78797308665256</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>47.81926196778836</v>
+        <v>27.29103883494373</v>
       </c>
     </row>
     <row r="5">
@@ -505,13 +505,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>83.09707998985907</v>
+        <v>77.89450671622312</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>27.96391793671203</v>
+        <v>25.30434767433095</v>
       </c>
     </row>
     <row r="6">
@@ -519,13 +519,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>63.7186528847603</v>
+        <v>80.18663264940636</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>37.79609048470516</v>
+        <v>31.22247777202508</v>
       </c>
     </row>
     <row r="7">
@@ -533,13 +533,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>71.23479869481011</v>
+        <v>78.67380464322395</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>25.31468801903539</v>
+        <v>43.3709695614556</v>
       </c>
     </row>
     <row r="8">
@@ -547,13 +547,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>73.61731565259345</v>
+        <v>66.91278582299184</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>20.82191331595294</v>
+        <v>37.192634535422</v>
       </c>
     </row>
     <row r="9">
@@ -561,13 +561,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>70.78146322440479</v>
+        <v>73.06792675889493</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>50.16767119380519</v>
+        <v>49.02513095017373</v>
       </c>
     </row>
     <row r="10">
@@ -575,13 +575,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>87.74275285989015</v>
+        <v>79.39998181218731</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>37.01703345467151</v>
+        <v>42.94691025191071</v>
       </c>
     </row>
     <row r="11">
@@ -589,13 +589,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>65.07725777705893</v>
+        <v>85.67064072789451</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>18.92773769807461</v>
+        <v>28.67636004871204</v>
       </c>
     </row>
     <row r="12">
@@ -603,13 +603,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>84.18389461883854</v>
+        <v>98.49683306895864</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>32.48013797558948</v>
+        <v>11.93995934113305</v>
       </c>
     </row>
     <row r="13">
@@ -617,13 +617,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>84.09769116136376</v>
+        <v>79.53810099541919</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>42.10087373196664</v>
+        <v>39.29526731666323</v>
       </c>
     </row>
     <row r="14">
@@ -631,13 +631,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>53.41095777554392</v>
+        <v>87.19993144819773</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>46.70020264959377</v>
+        <v>23.86745210635676</v>
       </c>
     </row>
     <row r="15">
@@ -645,13 +645,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>76.80863064009743</v>
+        <v>65.44044687503762</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>30.27835830246625</v>
+        <v>25.21790593515014</v>
       </c>
     </row>
     <row r="16">
@@ -659,13 +659,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>72.20924158141578</v>
+        <v>71.84326267416424</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>37.47606163303947</v>
+        <v>14.84019685560009</v>
       </c>
     </row>
     <row r="17">
@@ -673,13 +673,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>63.4947953640909</v>
+        <v>76.14748955654454</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>20.22874134428619</v>
+        <v>46.09185835416449</v>
       </c>
     </row>
     <row r="18">
@@ -687,13 +687,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>86.50680160591641</v>
+        <v>63.85044494966536</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>43.79122922720687</v>
+        <v>24.97625420114282</v>
       </c>
     </row>
     <row r="19">
@@ -701,13 +701,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>78.28930487092752</v>
+        <v>73.61156362749315</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>26.19318912777108</v>
+        <v>58.44727578702815</v>
       </c>
     </row>
     <row r="20">
@@ -715,13 +715,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>61.16937452653605</v>
+        <v>73.69808077401393</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>33.29926720781165</v>
+        <v>31.06762795859909</v>
       </c>
     </row>
     <row r="21">
@@ -729,13 +729,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>65.35430493132003</v>
+        <v>72.77464540928813</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>44.35265564626028</v>
+        <v>24.71704792280711</v>
       </c>
     </row>
     <row r="22">
@@ -743,13 +743,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>82.2215658668943</v>
+        <v>78.13821458469413</v>
       </c>
       <c r="C22" t="n">
         <v>21</v>
       </c>
       <c r="D22" t="n">
-        <v>38.23854664125035</v>
+        <v>34.3004928340894</v>
       </c>
     </row>
     <row r="23">
@@ -757,13 +757,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>68.78449716220743</v>
+        <v>82.54921766334198</v>
       </c>
       <c r="C23" t="n">
         <v>22</v>
       </c>
       <c r="D23" t="n">
-        <v>34.26100335248395</v>
+        <v>35.63726519650231</v>
       </c>
     </row>
     <row r="24">
@@ -771,13 +771,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>62.84382071551743</v>
+        <v>66.81614062508535</v>
       </c>
       <c r="C24" t="n">
         <v>23</v>
       </c>
       <c r="D24" t="n">
-        <v>45.07265708968812</v>
+        <v>21.84980794557303</v>
       </c>
     </row>
     <row r="25">
@@ -785,13 +785,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>61.39654528798138</v>
+        <v>69.14685534548096</v>
       </c>
       <c r="C25" t="n">
         <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>33.55445371607875</v>
+        <v>36.34352137331831</v>
       </c>
     </row>
     <row r="26">
@@ -799,13 +799,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>74.51230855430882</v>
+        <v>71.76988510977998</v>
       </c>
       <c r="C26" t="n">
         <v>25</v>
       </c>
       <c r="D26" t="n">
-        <v>46.80194324645724</v>
+        <v>26.18699762168223</v>
       </c>
     </row>
   </sheetData>
@@ -854,13 +854,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>7670.849727980974</v>
+        <v>7926.475314037275</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>7786.008131453756</v>
+        <v>7702.544120319138</v>
       </c>
     </row>
     <row r="3">
@@ -868,13 +868,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>7839.553860100211</v>
+        <v>7808.413349038202</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>7930.746276599633</v>
+        <v>7570.820436977559</v>
       </c>
     </row>
     <row r="4">
@@ -882,13 +882,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>7896.986428762432</v>
+        <v>7860.523244718825</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>7635.411153064268</v>
+        <v>7689.549832960259</v>
       </c>
     </row>
     <row r="5">
@@ -896,13 +896,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>6736.420690021456</v>
+        <v>7430.593747130135</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>6738.798679690955</v>
+        <v>7294.85251315582</v>
       </c>
     </row>
     <row r="6">
@@ -910,13 +910,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>7869.557453601535</v>
+        <v>7718.163871095317</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>7843.069961535311</v>
+        <v>7785.900476010769</v>
       </c>
     </row>
     <row r="7">
@@ -924,13 +924,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>7046.854857798955</v>
+        <v>7736.534024686456</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>7868.352659180621</v>
+        <v>7811.470789233801</v>
       </c>
     </row>
     <row r="8">
@@ -938,13 +938,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>7775.476429794619</v>
+        <v>7631.270174779402</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>7696.245592668011</v>
+        <v>7888.675479763126</v>
       </c>
     </row>
     <row r="9">
@@ -952,13 +952,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>7755.924873889781</v>
+        <v>7649.576378307789</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>7761.573699518959</v>
+        <v>7759.374707362307</v>
       </c>
     </row>
     <row r="10">
@@ -966,13 +966,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>7591.248917543384</v>
+        <v>7796.940217495404</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>7266.450565672319</v>
+        <v>7666.502788356008</v>
       </c>
     </row>
     <row r="11">
@@ -980,13 +980,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>7631.941456554055</v>
+        <v>7065.335045356524</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>7881.859499700697</v>
+        <v>7944.339622893721</v>
       </c>
     </row>
     <row r="12">
@@ -994,13 +994,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>7082.025346454595</v>
+        <v>7526.065655525987</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>7365.598187607988</v>
+        <v>7395.71150669999</v>
       </c>
     </row>
     <row r="13">
@@ -1008,13 +1008,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>7381.660580233637</v>
+        <v>7869.876153465468</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>7751.166957167938</v>
+        <v>7441.339447049034</v>
       </c>
     </row>
     <row r="14">
@@ -1022,13 +1022,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>7624.744707497926</v>
+        <v>7894.752875065903</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>7918.685829140993</v>
+        <v>7509.602906017682</v>
       </c>
     </row>
     <row r="15">
@@ -1036,13 +1036,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>6499.744225423534</v>
+        <v>7987.788046283485</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>7320.772646146371</v>
+        <v>7566.056701597195</v>
       </c>
     </row>
     <row r="16">
@@ -1050,13 +1050,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>7901.897751089019</v>
+        <v>7942.560412131164</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>7572.168701810511</v>
+        <v>6985.860145606375</v>
       </c>
     </row>
     <row r="17">
@@ -1064,13 +1064,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>7321.041986935189</v>
+        <v>7958.355272140101</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>7104.112623935078</v>
+        <v>7506.592527571425</v>
       </c>
     </row>
     <row r="18">
@@ -1078,13 +1078,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>7669.954099645398</v>
+        <v>7944.670388187845</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>7901.469787517514</v>
+        <v>7686.617828702971</v>
       </c>
     </row>
     <row r="19">
@@ -1092,13 +1092,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>7866.154589076468</v>
+        <v>7536.071838285672</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>6861.10383664087</v>
+        <v>7379.620248668145</v>
       </c>
     </row>
     <row r="20">
@@ -1106,13 +1106,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>7982.216554077999</v>
+        <v>7617.888560639178</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>6753.399774018735</v>
+        <v>7173.84841266849</v>
       </c>
     </row>
     <row r="21">
@@ -1120,13 +1120,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>7486.859344583012</v>
+        <v>7967.597512326689</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>7775.520950329103</v>
+        <v>7342.707536274914</v>
       </c>
     </row>
   </sheetData>
@@ -1175,13 +1175,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>0.8669000418115111</v>
+        <v>0.8527053013038211</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5344816371220522</v>
+        <v>0.5779572269019784</v>
       </c>
     </row>
     <row r="3">
@@ -1189,13 +1189,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8111448160986828</v>
+        <v>0.8703451844162384</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5018545418826674</v>
+        <v>0.5637416372645336</v>
       </c>
     </row>
     <row r="4">
@@ -1203,13 +1203,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.866390509303972</v>
+        <v>0.8688600047893295</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5244599367168462</v>
+        <v>0.5688678924436006</v>
       </c>
     </row>
     <row r="5">
@@ -1217,13 +1217,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.8343524574238459</v>
+        <v>0.8388035474242954</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>0.5193582296050649</v>
+        <v>0.5670420022040954</v>
       </c>
     </row>
     <row r="6">
@@ -1231,13 +1231,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8669649014059136</v>
+        <v>0.8079434983295667</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>0.5266023898763372</v>
+        <v>0.5191308701314556</v>
       </c>
     </row>
     <row r="7">
@@ -1245,13 +1245,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.8363924618911617</v>
+        <v>0.8027994267421097</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5923377031738626</v>
+        <v>0.5318751864437739</v>
       </c>
     </row>
     <row r="8">
@@ -1259,13 +1259,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.8233685019279536</v>
+        <v>0.8811963577885226</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5081204926888248</v>
+        <v>0.5888161826510172</v>
       </c>
     </row>
     <row r="9">
@@ -1273,13 +1273,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.8726878039822333</v>
+        <v>0.8185469622783554</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>0.5834013385360847</v>
+        <v>0.5342678943054601</v>
       </c>
     </row>
     <row r="10">
@@ -1287,13 +1287,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.8552210796272611</v>
+        <v>0.8942854485179723</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5019660249534544</v>
+        <v>0.5039955843865416</v>
       </c>
     </row>
     <row r="11">
@@ -1301,13 +1301,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.89716609122131</v>
+        <v>0.8424216513094339</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5028313524348221</v>
+        <v>0.584201885106019</v>
       </c>
     </row>
     <row r="12">
@@ -1315,13 +1315,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>0.8709698695777164</v>
+        <v>0.8952518636906553</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5962914138674927</v>
+        <v>0.5144646880629308</v>
       </c>
     </row>
     <row r="13">
@@ -1329,13 +1329,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>0.83157529835301</v>
+        <v>0.889888718213254</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5539081401270842</v>
+        <v>0.5662567941395467</v>
       </c>
     </row>
     <row r="14">
@@ -1343,13 +1343,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.8211682856157061</v>
+        <v>0.8107799411758587</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
       </c>
       <c r="D14" t="n">
-        <v>0.5474254482241685</v>
+        <v>0.5287013953536635</v>
       </c>
     </row>
     <row r="15">
@@ -1357,13 +1357,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.8240967467226784</v>
+        <v>0.8909007337621226</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>0.5919359941631341</v>
+        <v>0.5612085216917156</v>
       </c>
     </row>
     <row r="16">
@@ -1371,13 +1371,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>0.8289548331299081</v>
+        <v>0.8865039969472478</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
       </c>
       <c r="D16" t="n">
-        <v>0.5536565663790451</v>
+        <v>0.5115301341523676</v>
       </c>
     </row>
     <row r="17">
@@ -1385,13 +1385,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>0.8621366096020281</v>
+        <v>0.8465021522453199</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>0.5230679692918924</v>
+        <v>0.5152514107261935</v>
       </c>
     </row>
     <row r="18">
@@ -1399,13 +1399,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>0.8944371439060989</v>
+        <v>0.8332481311013943</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5841997097660503</v>
+        <v>0.5668118313403178</v>
       </c>
     </row>
     <row r="19">
@@ -1413,13 +1413,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>0.8970864450667373</v>
+        <v>0.8270069314228267</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>0.5909989160872702</v>
+        <v>0.5440821245922401</v>
       </c>
     </row>
     <row r="20">
@@ -1427,13 +1427,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>0.8939511512807504</v>
+        <v>0.8204585909095117</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>0.5011323243985301</v>
+        <v>0.5631049456719771</v>
       </c>
     </row>
     <row r="21">
@@ -1441,13 +1441,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>0.886760507231459</v>
+        <v>0.8064376077237216</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>0.5537661016152468</v>
+        <v>0.5062002051176431</v>
       </c>
     </row>
     <row r="22">
@@ -1455,13 +1455,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>0.8862258104538903</v>
+        <v>0.8456732594411598</v>
       </c>
       <c r="C22" t="n">
         <v>21</v>
       </c>
       <c r="D22" t="n">
-        <v>0.576069603779173</v>
+        <v>0.5828328296472806</v>
       </c>
     </row>
     <row r="23">
@@ -1469,13 +1469,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>0.8194186760563227</v>
+        <v>0.8234477651633498</v>
       </c>
       <c r="C23" t="n">
         <v>22</v>
       </c>
       <c r="D23" t="n">
-        <v>0.5824252951294644</v>
+        <v>0.5005781784953076</v>
       </c>
     </row>
     <row r="24">
@@ -1483,13 +1483,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>0.8303386517533771</v>
+        <v>0.8744107961252375</v>
       </c>
       <c r="C24" t="n">
         <v>23</v>
       </c>
       <c r="D24" t="n">
-        <v>0.5768870941784824</v>
+        <v>0.5545426106208231</v>
       </c>
     </row>
     <row r="25">
@@ -1497,13 +1497,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>0.8094030056144252</v>
+        <v>0.8385478968187281</v>
       </c>
       <c r="C25" t="n">
         <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>0.5106677397729527</v>
+        <v>0.5090494754095773</v>
       </c>
     </row>
     <row r="26">
@@ -1511,13 +1511,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>0.8417678346249561</v>
+        <v>0.8356484120577395</v>
       </c>
       <c r="C26" t="n">
         <v>25</v>
       </c>
       <c r="D26" t="n">
-        <v>0.5241948481021546</v>
+        <v>0.5261264432381142</v>
       </c>
     </row>
     <row r="27">
@@ -1525,13 +1525,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>0.8354107523962944</v>
+        <v>0.8260589285837828</v>
       </c>
       <c r="C27" t="n">
         <v>26</v>
       </c>
       <c r="D27" t="n">
-        <v>0.5903434150491226</v>
+        <v>0.5561070607683961</v>
       </c>
     </row>
     <row r="28">
@@ -1539,13 +1539,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>0.8893642414095376</v>
+        <v>0.8363020198665265</v>
       </c>
       <c r="C28" t="n">
         <v>27</v>
       </c>
       <c r="D28" t="n">
-        <v>0.554751323035479</v>
+        <v>0.5986254457732538</v>
       </c>
     </row>
     <row r="29">
@@ -1553,13 +1553,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>0.8133459655823825</v>
+        <v>0.8903258825256608</v>
       </c>
       <c r="C29" t="n">
         <v>28</v>
       </c>
       <c r="D29" t="n">
-        <v>0.5349588467409012</v>
+        <v>0.5028793475387421</v>
       </c>
     </row>
     <row r="30">
@@ -1567,13 +1567,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>0.8608056037748639</v>
+        <v>0.8161426905446616</v>
       </c>
       <c r="C30" t="n">
         <v>29</v>
       </c>
       <c r="D30" t="n">
-        <v>0.5671532254619741</v>
+        <v>0.5860557386440746</v>
       </c>
     </row>
     <row r="31">
@@ -1581,13 +1581,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>0.8186369116592933</v>
+        <v>0.8652451573250242</v>
       </c>
       <c r="C31" t="n">
         <v>30</v>
       </c>
       <c r="D31" t="n">
-        <v>0.5404886120693058</v>
+        <v>0.515872016529307</v>
       </c>
     </row>
     <row r="32">
@@ -1595,13 +1595,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>0.8232446756988376</v>
+        <v>0.8212469019581342</v>
       </c>
       <c r="C32" t="n">
         <v>31</v>
       </c>
       <c r="D32" t="n">
-        <v>0.5172487217728502</v>
+        <v>0.5617507785260554</v>
       </c>
     </row>
     <row r="33">
@@ -1609,13 +1609,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>0.8291769694151093</v>
+        <v>0.8684219769275475</v>
       </c>
       <c r="C33" t="n">
         <v>32</v>
       </c>
       <c r="D33" t="n">
-        <v>0.5041364146982324</v>
+        <v>0.5021781793642756</v>
       </c>
     </row>
     <row r="34">
@@ -1623,13 +1623,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>0.8311120790166713</v>
+        <v>0.8443576189902048</v>
       </c>
       <c r="C34" t="n">
         <v>33</v>
       </c>
       <c r="D34" t="n">
-        <v>0.5698087597126311</v>
+        <v>0.5453900924069252</v>
       </c>
     </row>
     <row r="35">
@@ -1637,13 +1637,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>0.885214558986105</v>
+        <v>0.8821932837813615</v>
       </c>
       <c r="C35" t="n">
         <v>34</v>
       </c>
       <c r="D35" t="n">
-        <v>0.5267040774995533</v>
+        <v>0.5644120119944833</v>
       </c>
     </row>
     <row r="36">
@@ -1651,13 +1651,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>0.8549856502986842</v>
+        <v>0.8690118670344305</v>
       </c>
       <c r="C36" t="n">
         <v>35</v>
       </c>
       <c r="D36" t="n">
-        <v>0.5054224103846067</v>
+        <v>0.585377934907354</v>
       </c>
     </row>
     <row r="37">
@@ -1665,13 +1665,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>0.8589022566631083</v>
+        <v>0.8782544448387986</v>
       </c>
       <c r="C37" t="n">
         <v>36</v>
       </c>
       <c r="D37" t="n">
-        <v>0.5171754412046695</v>
+        <v>0.519726331478139</v>
       </c>
     </row>
     <row r="38">
@@ -1679,13 +1679,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>0.86516146997175</v>
+        <v>0.8149800380873693</v>
       </c>
       <c r="C38" t="n">
         <v>37</v>
       </c>
       <c r="D38" t="n">
-        <v>0.5970111276673999</v>
+        <v>0.5926327843792362</v>
       </c>
     </row>
     <row r="39">
@@ -1693,13 +1693,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>0.8104532239530559</v>
+        <v>0.8658023731030191</v>
       </c>
       <c r="C39" t="n">
         <v>38</v>
       </c>
       <c r="D39" t="n">
-        <v>0.5454447961603374</v>
+        <v>0.5594631757144076</v>
       </c>
     </row>
     <row r="40">
@@ -1707,13 +1707,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>0.8879369800786422</v>
+        <v>0.8609858626782979</v>
       </c>
       <c r="C40" t="n">
         <v>39</v>
       </c>
       <c r="D40" t="n">
-        <v>0.5065508412852862</v>
+        <v>0.5193815253833143</v>
       </c>
     </row>
     <row r="41">
@@ -1721,13 +1721,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>0.803322716392506</v>
+        <v>0.8391207985090686</v>
       </c>
       <c r="C41" t="n">
         <v>40</v>
       </c>
       <c r="D41" t="n">
-        <v>0.5930523726155574</v>
+        <v>0.5781314456275051</v>
       </c>
     </row>
   </sheetData>
@@ -1776,13 +1776,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
@@ -1790,7 +1790,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
@@ -1804,13 +1804,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="C4" t="n">
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
@@ -1818,13 +1818,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
@@ -1832,13 +1832,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
         <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
@@ -1846,13 +1846,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>25</v>
+        <v>-0</v>
       </c>
       <c r="C7" t="n">
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -1860,13 +1860,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="C8" t="n">
         <v>7</v>
       </c>
       <c r="D8" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
@@ -1874,13 +1874,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
       </c>
       <c r="D9" t="n">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
@@ -1888,7 +1888,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
         <v>9</v>
@@ -1902,13 +1902,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>22</v>
+        <v>-0</v>
       </c>
       <c r="C11" t="n">
         <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12">
@@ -1916,13 +1916,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>26</v>
+        <v>-0</v>
       </c>
       <c r="C12" t="n">
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
@@ -1930,13 +1930,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14">
@@ -1944,7 +1944,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C14" t="n">
         <v>13</v>
@@ -1958,13 +1958,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>25</v>
+        <v>-0</v>
       </c>
       <c r="C15" t="n">
         <v>14</v>
       </c>
       <c r="D15" t="n">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16">
@@ -1972,7 +1972,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C16" t="n">
         <v>15</v>
@@ -1986,13 +1986,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C17" t="n">
         <v>16</v>
       </c>
       <c r="D17" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18">
@@ -2000,13 +2000,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C18" t="n">
         <v>17</v>
       </c>
       <c r="D18" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19">
@@ -2014,13 +2014,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="C19" t="n">
         <v>18</v>
       </c>
       <c r="D19" t="n">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20">
@@ -2028,13 +2028,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C20" t="n">
         <v>19</v>
       </c>
       <c r="D20" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21">
@@ -2042,13 +2042,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22">
@@ -2056,13 +2056,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="C22" t="n">
         <v>21</v>
       </c>
       <c r="D22" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23">
@@ -2070,13 +2070,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C23" t="n">
         <v>22</v>
       </c>
       <c r="D23" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24">
@@ -2084,13 +2084,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C24" t="n">
         <v>23</v>
       </c>
       <c r="D24" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25">
@@ -2098,13 +2098,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="C25" t="n">
         <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26">
@@ -2112,13 +2112,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="C26" t="n">
         <v>25</v>
       </c>
       <c r="D26" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>